<commit_message>
next/previous navigation added (testing)
</commit_message>
<xml_diff>
--- a/Key for data columns.xlsx
+++ b/Key for data columns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\code\croma\crowdinc.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BBACC4-6371-451F-A693-70D6C7A187EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03E211F-D444-4D23-AED5-CB3F2C03A4DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{B5A19073-F3C7-47B8-9EE7-17758FF8F12C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>Data 1</t>
   </si>
@@ -57,9 +57,6 @@
     <t>codeSnippet</t>
   </si>
   <si>
-    <t>next</t>
-  </si>
-  <si>
     <t>noteMove</t>
   </si>
   <si>
@@ -133,6 +130,12 @@
   </si>
   <si>
     <t>pattern</t>
+  </si>
+  <si>
+    <t>newFollow</t>
+  </si>
+  <si>
+    <t>direction (forward/backward)</t>
   </si>
 </sst>
 </file>
@@ -487,13 +490,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.15625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.3671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.89453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -517,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -531,27 +534,27 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -559,13 +562,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -573,13 +576,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -587,153 +590,153 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -741,27 +744,27 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began updating data logger for rt mingle
</commit_message>
<xml_diff>
--- a/Key for data columns.xlsx
+++ b/Key for data columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\code\croma\crowdinc.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03E211F-D444-4D23-AED5-CB3F2C03A4DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E50D09-609F-4F6E-A231-FDDCBB6D3579}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{B5A19073-F3C7-47B8-9EE7-17758FF8F12C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>Data 1</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>direction (forward/backward)</t>
+  </si>
+  <si>
+    <t>sendRequest</t>
+  </si>
+  <si>
+    <t>recipient</t>
+  </si>
+  <si>
+    <t>cancelRequest</t>
+  </si>
+  <si>
+    <t>ignoreRequest</t>
+  </si>
+  <si>
+    <t>acceptRequest</t>
   </si>
 </sst>
 </file>
@@ -487,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA7435-1A47-4C19-930B-C0B3E8E4E21B}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -767,6 +782,62 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D19">
     <sortCondition ref="A2:A19"/>

</xml_diff>

<commit_message>
slight wording change to log key
</commit_message>
<xml_diff>
--- a/Key for data columns.xlsx
+++ b/Key for data columns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\code\croma\crowdinc.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E50D09-609F-4F6E-A231-FDDCBB6D3579}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522067EE-003F-470F-AB43-489683B6447A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{B5A19073-F3C7-47B8-9EE7-17758FF8F12C}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>newFollow</t>
   </si>
   <si>
-    <t>direction (forward/backward)</t>
-  </si>
-  <si>
     <t>sendRequest</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>acceptRequest</t>
+  </si>
+  <si>
+    <t>direction (next/prev)</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:D23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -647,7 +647,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -798,10 +798,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
@@ -839,7 +839,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
     <sortCondition ref="A2:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixes and improvements (see closed github issues. stateChange logging, distance logging, etc)
</commit_message>
<xml_diff>
--- a/Key for data columns.xlsx
+++ b/Key for data columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\code\croma\crowdinc.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522067EE-003F-470F-AB43-489683B6447A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C97CB-30A7-4BF6-BC8E-0FAAC4355366}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5430" xr2:uid="{B5A19073-F3C7-47B8-9EE7-17758FF8F12C}"/>
+    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{B5A19073-F3C7-47B8-9EE7-17758FF8F12C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -549,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>

</xml_diff>